<commit_message>
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C768917
</commit_message>
<xml_diff>
--- a/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G84" sqref="A81:G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,18 +2577,6 @@
       <c r="G80" s="10" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="9"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="9"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="9"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Usman - Global Pages project with new users added
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C773159
</commit_message>
<xml_diff>
--- a/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="286">
   <si>
     <t>UserName</t>
   </si>
@@ -838,6 +838,42 @@
   </si>
   <si>
     <t xml:space="preserve">AssetPageUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t>GlobalPagesUser1</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser2</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser3</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser4</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser5</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser6</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser5@mailinator.com</t>
+  </si>
+  <si>
+    <t>GlobalPagesUser6@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -1258,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:G113"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,6 +3377,108 @@
       </c>
       <c r="G113" s="10" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>274</v>
+      </c>
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>275</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>276</v>
+      </c>
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>277</v>
+      </c>
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G117" s="10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>278</v>
+      </c>
+      <c r="B118" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G118" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>279</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G119" s="10" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3421,9 +3559,15 @@
     <hyperlink ref="G110" r:id="rId74"/>
     <hyperlink ref="G113" r:id="rId75"/>
     <hyperlink ref="G111" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G114" r:id="rId77"/>
+    <hyperlink ref="G115" r:id="rId78"/>
+    <hyperlink ref="G116" r:id="rId79"/>
+    <hyperlink ref="G117" r:id="rId80"/>
+    <hyperlink ref="G118" r:id="rId81"/>
+    <hyperlink ref="G119" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix for GLPage_UKUS1 user
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C796816
</commit_message>
<xml_diff>
--- a/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
@@ -390,9 +390,6 @@
     <t>GlPage_UKUS1</t>
   </si>
   <si>
-    <t>Global_page1</t>
-  </si>
-  <si>
     <t>GLPAGE_UK_US_USER</t>
   </si>
   <si>
@@ -883,6 +880,9 @@
   </si>
   <si>
     <t>FSTestUser2</t>
+  </si>
+  <si>
+    <t>Global_page1!</t>
   </si>
 </sst>
 </file>
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1915,10 +1915,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
@@ -2255,67 +2255,67 @@
         <v>123</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>124</v>
+        <v>288</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="F49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="F50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>52</v>
@@ -2329,12 +2329,12 @@
         <v>25</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2348,12 +2348,12 @@
         <v>25</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>52</v>
@@ -2361,1152 +2361,1152 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B80" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B81" t="s">
         <v>52</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="B82" t="s">
-        <v>52</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>209</v>
-      </c>
-      <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B84" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="B84" t="s">
-        <v>52</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="B85" t="s">
-        <v>52</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="B86" t="s">
-        <v>52</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B87" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G87" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="B87" t="s">
-        <v>52</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G87" s="10" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B88" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="B88" t="s">
-        <v>52</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G88" s="10" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="B89" t="s">
-        <v>52</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G89" s="10" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="B90" t="s">
-        <v>52</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" s="10" t="s">
         <v>225</v>
-      </c>
-      <c r="B91" t="s">
-        <v>52</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B92" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" s="10" t="s">
         <v>227</v>
-      </c>
-      <c r="B92" t="s">
-        <v>52</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G92" s="10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B93" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G93" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="B93" t="s">
-        <v>52</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G93" s="10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B94" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="10" t="s">
         <v>231</v>
-      </c>
-      <c r="B94" t="s">
-        <v>52</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G94" s="10" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" s="10" t="s">
         <v>233</v>
-      </c>
-      <c r="B95" t="s">
-        <v>52</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" s="10" t="s">
         <v>235</v>
-      </c>
-      <c r="B96" t="s">
-        <v>52</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B97" t="s">
-        <v>52</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G97" s="10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B98" t="s">
+        <v>52</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" s="10" t="s">
         <v>239</v>
-      </c>
-      <c r="B98" t="s">
-        <v>52</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G98" s="10" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" s="10" t="s">
         <v>241</v>
-      </c>
-      <c r="B99" t="s">
-        <v>52</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G99" s="10" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B100" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="B100" t="s">
-        <v>52</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G100" s="10" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B101" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G101" s="10" t="s">
         <v>245</v>
-      </c>
-      <c r="B101" t="s">
-        <v>52</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G101" s="10" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B102" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" s="10" t="s">
         <v>247</v>
-      </c>
-      <c r="B102" t="s">
-        <v>52</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G103" s="10" t="s">
         <v>249</v>
-      </c>
-      <c r="B103" t="s">
-        <v>52</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G103" s="10" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="B104" t="s">
-        <v>52</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G104" s="10" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G105" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="B105" t="s">
-        <v>52</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G105" s="10" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" s="10" t="s">
         <v>255</v>
-      </c>
-      <c r="B106" t="s">
-        <v>52</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F106" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G106" s="10" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G107" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="B107" t="s">
-        <v>52</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F107" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G107" s="10" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G108" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="B108" t="s">
-        <v>52</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G108" s="10" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G109" s="10" t="s">
         <v>261</v>
-      </c>
-      <c r="B109" t="s">
-        <v>52</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F109" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G109" s="10" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G110" s="10" t="s">
         <v>263</v>
-      </c>
-      <c r="B110" t="s">
-        <v>52</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G110" s="10" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G111" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="B111" t="s">
-        <v>52</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G111" s="10" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G112" s="10" t="s">
         <v>267</v>
-      </c>
-      <c r="B112" t="s">
-        <v>52</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G112" s="10" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" s="10" t="s">
         <v>269</v>
-      </c>
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G113" s="10" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="B114" t="s">
-        <v>52</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G114" s="10" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B115" t="s">
         <v>52</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F115" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G115" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B116" t="s">
         <v>52</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F116" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G116" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B117" t="s">
         <v>52</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F117" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B118" t="s">
         <v>52</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F118" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G118" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B119" t="s">
         <v>52</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F119" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B120" t="s">
         <v>52</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F120" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G120" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3618,23 +3618,23 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" t="s">
         <v>204</v>
-      </c>
-      <c r="B2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3652,7 +3652,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix GP user again
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C797184
</commit_message>
<xml_diff>
--- a/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-GlobalPages/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="288">
   <si>
     <t>UserName</t>
   </si>
@@ -387,9 +387,6 @@
     <t>ANZ history, please don't clean history!</t>
   </si>
   <si>
-    <t>GlPage_UKUS1</t>
-  </si>
-  <si>
     <t>GLPAGE_UK_US_USER</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
     <t>anztestuser4@mailinator.com</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Linking_AutoUser</t>
   </si>
   <si>
@@ -882,7 +876,10 @@
     <t>FSTestUser2</t>
   </si>
   <si>
-    <t>Global_page111!</t>
+    <t>GlPage_UKUS2</t>
+  </si>
+  <si>
+    <t>Global_page123!</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1303,7 @@
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,10 +1484,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1915,10 +1912,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
@@ -2252,70 +2249,70 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>123</v>
+        <v>286</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="F49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="F50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>52</v>
@@ -2329,12 +2326,12 @@
         <v>25</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2348,12 +2345,12 @@
         <v>25</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>52</v>
@@ -2361,1152 +2358,1152 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
         <v>52</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B82" t="s">
         <v>52</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B83" t="s">
         <v>52</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B84" t="s">
         <v>52</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F84" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F85" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F86" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B87" t="s">
         <v>52</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F87" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B88" t="s">
         <v>52</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F88" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F90" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F91" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F92" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F93" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B94" t="s">
         <v>52</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F94" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F95" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F96" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F97" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F98" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F99" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B100" t="s">
         <v>52</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F100" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B101" t="s">
         <v>52</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F101" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F102" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F103" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F104" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B105" t="s">
         <v>52</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F105" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B106" t="s">
         <v>52</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F106" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F107" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B108" t="s">
         <v>52</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F108" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B109" t="s">
         <v>52</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F109" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F111" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F112" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B113" t="s">
         <v>52</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F113" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G113" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B114" t="s">
         <v>52</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F114" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G114" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B115" t="s">
         <v>52</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F115" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G115" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B116" t="s">
         <v>52</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F116" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G116" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B117" t="s">
         <v>52</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F117" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B118" t="s">
         <v>52</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F118" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G118" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B119" t="s">
         <v>52</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F119" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B120" t="s">
         <v>52</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F120" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G120" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3609,8 +3606,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3618,23 +3615,23 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3644,18 +3641,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>